<commit_message>
move validation sheet to another file
</commit_message>
<xml_diff>
--- a/Literature_review_data.xlsx
+++ b/Literature_review_data.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Razan\Bitbucket\mappingCTSEprops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9C5979-E056-4BB0-8633-1B09D5B4145A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F12E60-F454-46EF-B48E-82BC36AF95E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{93EA37D0-547C-4F6C-8D12-FC66693056E1}"/>
   </bookViews>
   <sheets>
     <sheet name="List of SEAMS publications" sheetId="1" r:id="rId1"/>
     <sheet name="Included papers extracted data" sheetId="2" r:id="rId2"/>
-    <sheet name="SE properties Validation" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Included papers extracted data'!$A$1:$T$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'List of SEAMS publications'!$A$1:$E$119</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -129,71 +128,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={4E8FC4C9-E846-4422-94C5-13617D5694A2}</author>
-    <author>tc={04A14B2C-5D68-49EE-854F-E945EB906C2A}</author>
-    <author>tc={6C72BA6E-103B-43FA-8252-7AA6DD2C004A}</author>
-    <author>tc={CCBA7123-0903-4766-AC8C-0764808E6564}</author>
-    <author>tc={5047B8C0-1FE2-4DE0-9EA2-CA7B086C5D99}</author>
-    <author>tc={90E4EBBD-3C6F-410D-B361-BE9AA3A0E1DC}</author>
-  </authors>
-  <commentList>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{4E8FC4C9-E846-4422-94C5-13617D5694A2}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</t>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="1" shapeId="0" xr:uid="{04A14B2C-5D68-49EE-854F-E945EB906C2A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Fuzzy behavior Temporal Logic</t>
-      </text>
-    </comment>
-    <comment ref="D14" authorId="2" shapeId="0" xr:uid="{6C72BA6E-103B-43FA-8252-7AA6DD2C004A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</t>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="3" shapeId="0" xr:uid="{CCBA7123-0903-4766-AC8C-0764808E6564}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</t>
-      </text>
-    </comment>
-    <comment ref="D16" authorId="4" shapeId="0" xr:uid="{5047B8C0-1FE2-4DE0-9EA2-CA7B086C5D99}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</t>
-      </text>
-    </comment>
-    <comment ref="D17" authorId="5" shapeId="0" xr:uid="{90E4EBBD-3C6F-410D-B361-BE9AA3A0E1DC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="596">
   <si>
     <t>ID</t>
   </si>
@@ -1990,271 +1926,13 @@
   </si>
   <si>
     <t>Safety (time constrained)</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>Meta</t>
-  </si>
-  <si>
-    <t>Property</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Decision</t>
-  </si>
-  <si>
-    <t>Who?</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Thorsten</t>
-  </si>
-  <si>
-    <t>EXCLUDED IN THE DATA EXTRACTION PROCESS, PLEASE READ THE COMMENT -&gt;</t>
-  </si>
-  <si>
-    <t>There is no explicit property formalism that is used with/against a model to synthesize or rverify something. The authors propose a reduction o the overhead of runtime monitoring based on a DSL that uses set-based notation but do not provide models neither properties.</t>
-  </si>
-  <si>
-    <t>Despite the use of PRISM to synthesize plans dynamic plans, it is a short paper that does not specify properties formalism and keeps models at a shallow level.</t>
-  </si>
-  <si>
-    <t>The paper presents a UPPAAL model and defines the property that is verified using natural language. Since the verification process is delegated to the ActivFORMS, as a reference, there is no sufficient information to collect from this paper.</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Sect 3 exmpl</t>
-  </si>
-  <si>
-    <t>"(FB ∨ FC) ∧ (FD ∨ FE)"</t>
-  </si>
-  <si>
-    <t>offline</t>
-  </si>
-  <si>
-    <t>Braking System</t>
-  </si>
-  <si>
-    <t>Indeed, the paper presents a formalization and composition of features based on goal model refinement operations. The authors generate monitors that awaits for the detection of feature interactions during runtime, to triggger the adaptation. However, I could not spot in the exmple, explicit formalization of the properties since they are encoded as the goal model of figure 4.  I would exlucde this paper since there is no explicit formalism for the property or the model.</t>
-  </si>
-  <si>
-    <t>Utilitarian(reliability)</t>
-  </si>
-  <si>
-    <t>Section 3.1</t>
-  </si>
-  <si>
-    <t>Egalitarian(reliability)</t>
-  </si>
-  <si>
-    <t>Nash(reliability)</t>
-  </si>
-  <si>
-    <t>Processor use rate(overloaded)</t>
-  </si>
-  <si>
-    <t>Section 3.2</t>
-  </si>
-  <si>
-    <t>Memory use rate(overloaded)</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Reconsider Table 2</t>
-  </si>
-  <si>
-    <t>Patrizio</t>
-  </si>
-  <si>
-    <t>FBTL</t>
-  </si>
-  <si>
-    <t>Table 3. R1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "f ailurerate &lt;= 0.15"</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>Non-subjective and quantitative reasoning</t>
-  </si>
-  <si>
-    <t>Health Care (Service)</t>
-  </si>
-  <si>
-    <t>The authors use DeSiRE to formalize some properties but do not make explicit how they use these properties in the adaptation engines.</t>
-  </si>
-  <si>
-    <t>Table 3. R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "cost &lt;= 8"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 3. R3. </t>
-  </si>
-  <si>
-    <t>"ervicetime &lt;= 80"</t>
-  </si>
-  <si>
-    <t>Optimization</t>
-  </si>
-  <si>
-    <t>Table 4. R1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Packet loss shall be as low as possible."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IoT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 4. R2. </t>
-  </si>
-  <si>
-    <t>"Energy consumption shall be as low as possible"</t>
-  </si>
-  <si>
-    <t>Reconsider properties</t>
-  </si>
-  <si>
-    <t>Architeture</t>
-  </si>
-  <si>
-    <t>Should we include this? Utility Function</t>
-  </si>
-  <si>
-    <t>The authors propose Q-learning as means of synthesizng an adaptive controller capable of guaranteeing timing constraints. Yet, no property was formalized.</t>
-  </si>
-  <si>
-    <t>highlight that the analysis is for a family of products, to analyze all the configurations simultaneously to speed up the analysis.</t>
-  </si>
-  <si>
-    <t>Quality of service estimation for DSPL configurations</t>
-  </si>
-  <si>
-    <t>runtime</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>Damage Spread</t>
-  </si>
-  <si>
-    <t>Power Cascade</t>
-  </si>
-  <si>
-    <t>Damage Correlation</t>
-  </si>
-  <si>
-    <t>Not sure the paper should be excluded. They are not super clear on specifying properties, but these are some of them</t>
-  </si>
-  <si>
-    <t>Ricardo: "I could not spot properties, models or any formalisms."</t>
-  </si>
-  <si>
-    <t>Reconsider all</t>
-  </si>
-  <si>
-    <t>Danny</t>
-  </si>
-  <si>
-    <t>Check clients who reopen tickets frequently</t>
-  </si>
-  <si>
-    <t>Table 2.P1</t>
-  </si>
-  <si>
-    <t>Model checking to establish confidence intervals for model properties</t>
-  </si>
-  <si>
-    <t>IT ticket support system</t>
-  </si>
-  <si>
-    <t>support attendants with high rates of suspended tickets</t>
-  </si>
-  <si>
-    <t>Table 2.P2</t>
-  </si>
-  <si>
-    <t>Support users that cancel tickets Support without requiring more information</t>
-  </si>
-  <si>
-    <t>Support users that open tickets on behalf of clients where the ticket is subsequently abandoned</t>
-  </si>
-  <si>
-    <t>Suppport users with a high combined rate of suspended, canceled, reopened and reallocation tickets</t>
-  </si>
-  <si>
-    <t>Table 2.P5</t>
-  </si>
-  <si>
-    <t>Detect expensive clients  to the system</t>
-  </si>
-  <si>
-    <t>Table 2.P6</t>
-  </si>
-  <si>
-    <t>The paper is an exemplar, which is under our exclusion criteria</t>
-  </si>
-  <si>
-    <t>there is 1 more prop</t>
-  </si>
-  <si>
-    <t>ndicates that configuration c_x0002_ can be reached immediately from c through the use of an adaptation action"</t>
-  </si>
-  <si>
-    <t>Target System + Environment</t>
-  </si>
-  <si>
-    <t>ec1</t>
-  </si>
-  <si>
-    <t>The authors propose a formal model of hybrid planning. We are seeking the usage of formal methods for guaranteeing some properties in self-adaptive systems and the paper does apply the model to any problem, leaving it to future work.</t>
-  </si>
-  <si>
-    <t>Changed</t>
-  </si>
-  <si>
-    <t>There is no clear formalism for the properties. They said to be STO-reqs, the requirements are elicited but no properties specified.</t>
-  </si>
-  <si>
-    <t>same argument as shevtsov</t>
-  </si>
-  <si>
-    <t>The authors propose control theory design for guarantees assurance in a two phase approach: first control synthesis then parameters adjusting. Yet, there are no properties formalized and the models are analytical.</t>
-  </si>
-  <si>
-    <t>The authors use evolutionary algoriths for taming uncertainties described in goal models. No formalisms, really.</t>
-  </si>
-  <si>
-    <t>The authors idea is to use learning of adaptation rules at design time to anticipate runtime changes. The feature models are acoompained from some formalisms but are not necessarily using them for synthesis, verification, etc.</t>
-  </si>
-  <si>
-    <t>SE properties Validation</t>
-  </si>
-  <si>
-    <t>Exclude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2270,13 +1948,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2289,14 +1962,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2369,20 +2036,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2424,43 +2082,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -2822,36 +2450,11 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D13" dT="2020-12-17T06:48:55.05" personId="{A76E3C88-9401-4016-BAEC-8D918CBDCA0E}" id="{4E8FC4C9-E846-4422-94C5-13617D5694A2}">
-    <text>These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</text>
-  </threadedComment>
-  <threadedComment ref="G13" dT="2020-12-17T10:32:58.15" personId="{A76E3C88-9401-4016-BAEC-8D918CBDCA0E}" id="{04A14B2C-5D68-49EE-854F-E945EB906C2A}">
-    <text>Fuzzy behavior Temporal Logic</text>
-  </threadedComment>
-  <threadedComment ref="D14" dT="2020-12-17T06:48:55.05" personId="{A76E3C88-9401-4016-BAEC-8D918CBDCA0E}" id="{6C72BA6E-103B-43FA-8252-7AA6DD2C004A}">
-    <text>These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</text>
-  </threadedComment>
-  <threadedComment ref="D15" dT="2020-12-17T06:48:55.05" personId="{A76E3C88-9401-4016-BAEC-8D918CBDCA0E}" id="{CCBA7123-0903-4766-AC8C-0764808E6564}">
-    <text>These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</text>
-  </threadedComment>
-  <threadedComment ref="D16" dT="2020-12-17T06:48:55.05" personId="{A76E3C88-9401-4016-BAEC-8D918CBDCA0E}" id="{5047B8C0-1FE2-4DE0-9EA2-CA7B086C5D99}">
-    <text>These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</text>
-  </threadedComment>
-  <threadedComment ref="D17" dT="2020-12-17T06:48:55.05" personId="{A76E3C88-9401-4016-BAEC-8D918CBDCA0E}" id="{90E4EBBD-3C6F-410D-B361-BE9AA3A0E1DC}">
-    <text>These cases are quite curious. There is some formalization proposal but not explicit use against a model or so.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FDD316-7944-45A0-94A2-2098DC1645BB}">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4888,10 +4491,10 @@
   </sheetData>
   <autoFilter ref="A1:E119" xr:uid="{0BB33AAD-CF15-47CE-B03B-EED5EB97A192}"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Excluded"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Included"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4907,8 +4510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CCF711-4516-4809-827A-2B0BF844EAD5}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5230,7 +4833,7 @@
       <c r="P5" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="20" t="s">
         <v>299</v>
       </c>
       <c r="R5" t="s">
@@ -5336,7 +4939,7 @@
       <c r="J7" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="20" t="s">
         <v>313</v>
       </c>
       <c r="L7" t="s">
@@ -5398,7 +5001,7 @@
       <c r="J8" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="20" t="s">
         <v>320</v>
       </c>
       <c r="L8" t="s">
@@ -8160,1637 +7763,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191103B3-EA98-4620-A4F7-C6D836D632A5}">
-  <dimension ref="A1:R38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="8" width="19.88671875" customWidth="1"/>
-    <col min="9" max="9" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34" customWidth="1"/>
-    <col min="12" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="15" width="19.88671875" customWidth="1"/>
-    <col min="16" max="16" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.6640625" customWidth="1"/>
-    <col min="18" max="18" width="27.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>680</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-    </row>
-    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
-        <v>596</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23" t="s">
-        <v>597</v>
-      </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
-        <v>598</v>
-      </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23" t="s">
-        <v>599</v>
-      </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>600</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>601</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>591</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>681</v>
-      </c>
-      <c r="B4" t="s">
-        <v>603</v>
-      </c>
-      <c r="C4">
-        <v>2019</v>
-      </c>
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>681</v>
-      </c>
-      <c r="B5" t="s">
-        <v>603</v>
-      </c>
-      <c r="C5">
-        <v>2019</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>681</v>
-      </c>
-      <c r="B6" t="s">
-        <v>603</v>
-      </c>
-      <c r="C6">
-        <v>2019</v>
-      </c>
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>648</v>
-      </c>
-      <c r="B7" t="s">
-        <v>603</v>
-      </c>
-      <c r="C7">
-        <v>2018</v>
-      </c>
-      <c r="D7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" t="s">
-        <v>328</v>
-      </c>
-      <c r="F7" t="s">
-        <v>364</v>
-      </c>
-      <c r="G7" t="s">
-        <v>365</v>
-      </c>
-      <c r="H7" t="s">
-        <v>608</v>
-      </c>
-      <c r="I7" t="s">
-        <v>608</v>
-      </c>
-      <c r="J7" t="s">
-        <v>609</v>
-      </c>
-      <c r="K7" t="s">
-        <v>610</v>
-      </c>
-      <c r="L7" t="s">
-        <v>263</v>
-      </c>
-      <c r="M7" t="s">
-        <v>328</v>
-      </c>
-      <c r="O7" t="s">
-        <v>369</v>
-      </c>
-      <c r="P7" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>612</v>
-      </c>
-      <c r="R7" s="25" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>648</v>
-      </c>
-      <c r="B8" t="s">
-        <v>603</v>
-      </c>
-      <c r="C8">
-        <v>2018</v>
-      </c>
-      <c r="D8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" t="s">
-        <v>614</v>
-      </c>
-      <c r="G8" t="s">
-        <v>310</v>
-      </c>
-      <c r="H8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" t="s">
-        <v>371</v>
-      </c>
-      <c r="K8" t="s">
-        <v>615</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="O8" t="s">
-        <v>374</v>
-      </c>
-      <c r="P8" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>648</v>
-      </c>
-      <c r="B9" t="s">
-        <v>603</v>
-      </c>
-      <c r="C9">
-        <v>2018</v>
-      </c>
-      <c r="D9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" t="s">
-        <v>616</v>
-      </c>
-      <c r="G9" t="s">
-        <v>310</v>
-      </c>
-      <c r="H9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" t="s">
-        <v>371</v>
-      </c>
-      <c r="K9" t="s">
-        <v>615</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="O9" t="s">
-        <v>374</v>
-      </c>
-      <c r="P9" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>648</v>
-      </c>
-      <c r="B10" t="s">
-        <v>603</v>
-      </c>
-      <c r="C10">
-        <v>2018</v>
-      </c>
-      <c r="D10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" t="s">
-        <v>617</v>
-      </c>
-      <c r="G10" t="s">
-        <v>310</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" t="s">
-        <v>371</v>
-      </c>
-      <c r="K10" t="s">
-        <v>615</v>
-      </c>
-      <c r="L10" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="O10" t="s">
-        <v>374</v>
-      </c>
-      <c r="P10" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>648</v>
-      </c>
-      <c r="B11" t="s">
-        <v>603</v>
-      </c>
-      <c r="C11">
-        <v>2018</v>
-      </c>
-      <c r="D11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" t="s">
-        <v>618</v>
-      </c>
-      <c r="G11" t="s">
-        <v>310</v>
-      </c>
-      <c r="H11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" t="s">
-        <v>376</v>
-      </c>
-      <c r="K11" t="s">
-        <v>619</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="O11" t="s">
-        <v>374</v>
-      </c>
-      <c r="P11" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>648</v>
-      </c>
-      <c r="B12" t="s">
-        <v>603</v>
-      </c>
-      <c r="C12">
-        <v>2018</v>
-      </c>
-      <c r="D12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" t="s">
-        <v>620</v>
-      </c>
-      <c r="G12" t="s">
-        <v>310</v>
-      </c>
-      <c r="H12" t="s">
-        <v>621</v>
-      </c>
-      <c r="I12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" t="s">
-        <v>376</v>
-      </c>
-      <c r="K12" t="s">
-        <v>619</v>
-      </c>
-      <c r="L12" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="O12" t="s">
-        <v>374</v>
-      </c>
-      <c r="P12" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>622</v>
-      </c>
-      <c r="B13" t="s">
-        <v>623</v>
-      </c>
-      <c r="C13">
-        <v>2018</v>
-      </c>
-      <c r="D13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" t="s">
-        <v>345</v>
-      </c>
-      <c r="F13" t="s">
-        <v>274</v>
-      </c>
-      <c r="G13" t="s">
-        <v>624</v>
-      </c>
-      <c r="H13" t="s">
-        <v>608</v>
-      </c>
-      <c r="I13" t="s">
-        <v>608</v>
-      </c>
-      <c r="J13" t="s">
-        <v>625</v>
-      </c>
-      <c r="K13" t="s">
-        <v>626</v>
-      </c>
-      <c r="L13" t="s">
-        <v>263</v>
-      </c>
-      <c r="M13" t="s">
-        <v>627</v>
-      </c>
-      <c r="N13" t="s">
-        <v>627</v>
-      </c>
-      <c r="O13" t="s">
-        <v>628</v>
-      </c>
-      <c r="P13" t="s">
-        <v>627</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>629</v>
-      </c>
-      <c r="R13" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>622</v>
-      </c>
-      <c r="B14" t="s">
-        <v>623</v>
-      </c>
-      <c r="C14">
-        <v>2018</v>
-      </c>
-      <c r="D14" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" t="s">
-        <v>272</v>
-      </c>
-      <c r="F14" t="s">
-        <v>274</v>
-      </c>
-      <c r="G14" t="s">
-        <v>624</v>
-      </c>
-      <c r="H14" t="s">
-        <v>608</v>
-      </c>
-      <c r="I14" t="s">
-        <v>608</v>
-      </c>
-      <c r="J14" t="s">
-        <v>631</v>
-      </c>
-      <c r="K14" t="s">
-        <v>632</v>
-      </c>
-      <c r="L14" t="s">
-        <v>263</v>
-      </c>
-      <c r="M14" t="s">
-        <v>627</v>
-      </c>
-      <c r="N14" t="s">
-        <v>627</v>
-      </c>
-      <c r="O14" t="s">
-        <v>628</v>
-      </c>
-      <c r="P14" t="s">
-        <v>627</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>622</v>
-      </c>
-      <c r="B15" t="s">
-        <v>623</v>
-      </c>
-      <c r="C15">
-        <v>2018</v>
-      </c>
-      <c r="D15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" t="s">
-        <v>346</v>
-      </c>
-      <c r="F15" t="s">
-        <v>274</v>
-      </c>
-      <c r="G15" t="s">
-        <v>624</v>
-      </c>
-      <c r="H15" t="s">
-        <v>608</v>
-      </c>
-      <c r="I15" t="s">
-        <v>608</v>
-      </c>
-      <c r="J15" t="s">
-        <v>633</v>
-      </c>
-      <c r="K15" t="s">
-        <v>634</v>
-      </c>
-      <c r="L15" t="s">
-        <v>263</v>
-      </c>
-      <c r="M15" t="s">
-        <v>627</v>
-      </c>
-      <c r="N15" t="s">
-        <v>627</v>
-      </c>
-      <c r="O15" t="s">
-        <v>628</v>
-      </c>
-      <c r="P15" t="s">
-        <v>627</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>622</v>
-      </c>
-      <c r="B16" t="s">
-        <v>623</v>
-      </c>
-      <c r="C16">
-        <v>2018</v>
-      </c>
-      <c r="D16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" t="s">
-        <v>635</v>
-      </c>
-      <c r="F16" t="s">
-        <v>274</v>
-      </c>
-      <c r="G16" t="s">
-        <v>624</v>
-      </c>
-      <c r="H16" t="s">
-        <v>608</v>
-      </c>
-      <c r="I16" t="s">
-        <v>608</v>
-      </c>
-      <c r="J16" t="s">
-        <v>636</v>
-      </c>
-      <c r="K16" t="s">
-        <v>637</v>
-      </c>
-      <c r="L16" t="s">
-        <v>263</v>
-      </c>
-      <c r="M16" t="s">
-        <v>627</v>
-      </c>
-      <c r="N16" t="s">
-        <v>627</v>
-      </c>
-      <c r="O16" t="s">
-        <v>628</v>
-      </c>
-      <c r="P16" t="s">
-        <v>627</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>622</v>
-      </c>
-      <c r="B17" t="s">
-        <v>623</v>
-      </c>
-      <c r="C17">
-        <v>2018</v>
-      </c>
-      <c r="D17" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" t="s">
-        <v>635</v>
-      </c>
-      <c r="F17" t="s">
-        <v>274</v>
-      </c>
-      <c r="G17" t="s">
-        <v>624</v>
-      </c>
-      <c r="H17" t="s">
-        <v>608</v>
-      </c>
-      <c r="I17" t="s">
-        <v>608</v>
-      </c>
-      <c r="J17" t="s">
-        <v>639</v>
-      </c>
-      <c r="K17" t="s">
-        <v>640</v>
-      </c>
-      <c r="L17" t="s">
-        <v>263</v>
-      </c>
-      <c r="M17" t="s">
-        <v>627</v>
-      </c>
-      <c r="N17" t="s">
-        <v>627</v>
-      </c>
-      <c r="O17" t="s">
-        <v>628</v>
-      </c>
-      <c r="P17" t="s">
-        <v>627</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>641</v>
-      </c>
-      <c r="B18" t="s">
-        <v>623</v>
-      </c>
-      <c r="C18">
-        <v>2018</v>
-      </c>
-      <c r="D18" t="s">
-        <v>117</v>
-      </c>
-      <c r="L18" t="s">
-        <v>263</v>
-      </c>
-      <c r="M18" t="s">
-        <v>642</v>
-      </c>
-      <c r="O18" t="s">
-        <v>381</v>
-      </c>
-      <c r="P18" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>643</v>
-      </c>
-      <c r="B19" t="s">
-        <v>623</v>
-      </c>
-      <c r="C19">
-        <v>2018</v>
-      </c>
-      <c r="D19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>645</v>
-      </c>
-      <c r="B20" t="s">
-        <v>623</v>
-      </c>
-      <c r="C20">
-        <v>2018</v>
-      </c>
-      <c r="D20" t="s">
-        <v>133</v>
-      </c>
-      <c r="E20" t="s">
-        <v>415</v>
-      </c>
-      <c r="F20" t="s">
-        <v>364</v>
-      </c>
-      <c r="G20" t="s">
-        <v>365</v>
-      </c>
-      <c r="H20" t="s">
-        <v>608</v>
-      </c>
-      <c r="I20" t="s">
-        <v>608</v>
-      </c>
-      <c r="L20" t="s">
-        <v>263</v>
-      </c>
-      <c r="M20" t="s">
-        <v>418</v>
-      </c>
-      <c r="N20" t="s">
-        <v>305</v>
-      </c>
-      <c r="O20" t="s">
-        <v>646</v>
-      </c>
-      <c r="P20" t="s">
-        <v>647</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>648</v>
-      </c>
-      <c r="B21" t="s">
-        <v>623</v>
-      </c>
-      <c r="C21">
-        <v>2018</v>
-      </c>
-      <c r="D21" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" t="s">
-        <v>649</v>
-      </c>
-      <c r="F21" t="s">
-        <v>310</v>
-      </c>
-      <c r="G21" t="s">
-        <v>310</v>
-      </c>
-      <c r="H21" t="s">
-        <v>621</v>
-      </c>
-      <c r="I21" t="s">
-        <v>608</v>
-      </c>
-      <c r="J21" t="s">
-        <v>423</v>
-      </c>
-      <c r="K21" t="s">
-        <v>424</v>
-      </c>
-      <c r="L21" t="s">
-        <v>314</v>
-      </c>
-      <c r="M21" t="s">
-        <v>425</v>
-      </c>
-      <c r="N21" t="s">
-        <v>310</v>
-      </c>
-      <c r="O21" t="s">
-        <v>426</v>
-      </c>
-      <c r="P21" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>648</v>
-      </c>
-      <c r="B22" t="s">
-        <v>623</v>
-      </c>
-      <c r="C22">
-        <v>2018</v>
-      </c>
-      <c r="D22" t="s">
-        <v>138</v>
-      </c>
-      <c r="E22" t="s">
-        <v>650</v>
-      </c>
-      <c r="F22" t="s">
-        <v>310</v>
-      </c>
-      <c r="G22" t="s">
-        <v>310</v>
-      </c>
-      <c r="H22" t="s">
-        <v>608</v>
-      </c>
-      <c r="I22" t="s">
-        <v>621</v>
-      </c>
-      <c r="J22" t="s">
-        <v>428</v>
-      </c>
-      <c r="K22" t="s">
-        <v>429</v>
-      </c>
-      <c r="L22" t="s">
-        <v>314</v>
-      </c>
-      <c r="M22" t="s">
-        <v>425</v>
-      </c>
-      <c r="N22" t="s">
-        <v>310</v>
-      </c>
-      <c r="O22" t="s">
-        <v>426</v>
-      </c>
-      <c r="P22" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>648</v>
-      </c>
-      <c r="B23" t="s">
-        <v>623</v>
-      </c>
-      <c r="C23">
-        <v>2018</v>
-      </c>
-      <c r="D23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E23" t="s">
-        <v>651</v>
-      </c>
-      <c r="F23" t="s">
-        <v>310</v>
-      </c>
-      <c r="G23" t="s">
-        <v>310</v>
-      </c>
-      <c r="H23" t="s">
-        <v>608</v>
-      </c>
-      <c r="I23" t="s">
-        <v>608</v>
-      </c>
-      <c r="J23" t="s">
-        <v>430</v>
-      </c>
-      <c r="K23" t="s">
-        <v>431</v>
-      </c>
-      <c r="L23" t="s">
-        <v>314</v>
-      </c>
-      <c r="M23" t="s">
-        <v>425</v>
-      </c>
-      <c r="N23" t="s">
-        <v>310</v>
-      </c>
-      <c r="O23" t="s">
-        <v>426</v>
-      </c>
-      <c r="P23" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>652</v>
-      </c>
-      <c r="B24" t="s">
-        <v>623</v>
-      </c>
-      <c r="C24">
-        <v>2018</v>
-      </c>
-      <c r="D24" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>654</v>
-      </c>
-      <c r="B25" t="s">
-        <v>655</v>
-      </c>
-      <c r="C25">
-        <v>2017</v>
-      </c>
-      <c r="D25" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" t="s">
-        <v>656</v>
-      </c>
-      <c r="G25" t="s">
-        <v>275</v>
-      </c>
-      <c r="J25" t="s">
-        <v>657</v>
-      </c>
-      <c r="K25" t="s">
-        <v>464</v>
-      </c>
-      <c r="L25" t="s">
-        <v>465</v>
-      </c>
-      <c r="O25" t="s">
-        <v>658</v>
-      </c>
-      <c r="P25" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>654</v>
-      </c>
-      <c r="B26" t="s">
-        <v>655</v>
-      </c>
-      <c r="C26">
-        <v>2017</v>
-      </c>
-      <c r="D26" t="s">
-        <v>155</v>
-      </c>
-      <c r="E26" t="s">
-        <v>660</v>
-      </c>
-      <c r="G26" t="s">
-        <v>275</v>
-      </c>
-      <c r="J26" t="s">
-        <v>661</v>
-      </c>
-      <c r="K26" t="s">
-        <v>464</v>
-      </c>
-      <c r="L26" t="s">
-        <v>465</v>
-      </c>
-      <c r="O26" t="s">
-        <v>658</v>
-      </c>
-      <c r="P26" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>654</v>
-      </c>
-      <c r="B27" t="s">
-        <v>655</v>
-      </c>
-      <c r="C27">
-        <v>2017</v>
-      </c>
-      <c r="D27" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27" t="s">
-        <v>662</v>
-      </c>
-      <c r="G27" t="s">
-        <v>275</v>
-      </c>
-      <c r="J27" t="s">
-        <v>468</v>
-      </c>
-      <c r="K27" t="s">
-        <v>464</v>
-      </c>
-      <c r="L27" t="s">
-        <v>465</v>
-      </c>
-      <c r="O27" t="s">
-        <v>658</v>
-      </c>
-      <c r="P27" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>654</v>
-      </c>
-      <c r="B28" t="s">
-        <v>655</v>
-      </c>
-      <c r="C28">
-        <v>2017</v>
-      </c>
-      <c r="D28" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" t="s">
-        <v>663</v>
-      </c>
-      <c r="G28" t="s">
-        <v>275</v>
-      </c>
-      <c r="J28" t="s">
-        <v>472</v>
-      </c>
-      <c r="K28" t="s">
-        <v>464</v>
-      </c>
-      <c r="L28" t="s">
-        <v>465</v>
-      </c>
-      <c r="O28" t="s">
-        <v>658</v>
-      </c>
-      <c r="P28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>654</v>
-      </c>
-      <c r="B29" t="s">
-        <v>655</v>
-      </c>
-      <c r="C29">
-        <v>2017</v>
-      </c>
-      <c r="D29" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" t="s">
-        <v>664</v>
-      </c>
-      <c r="G29" t="s">
-        <v>275</v>
-      </c>
-      <c r="J29" t="s">
-        <v>665</v>
-      </c>
-      <c r="K29" t="s">
-        <v>464</v>
-      </c>
-      <c r="L29" t="s">
-        <v>465</v>
-      </c>
-      <c r="O29" t="s">
-        <v>658</v>
-      </c>
-      <c r="P29" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>654</v>
-      </c>
-      <c r="B30" t="s">
-        <v>655</v>
-      </c>
-      <c r="C30">
-        <v>2017</v>
-      </c>
-      <c r="D30" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" t="s">
-        <v>666</v>
-      </c>
-      <c r="G30" t="s">
-        <v>275</v>
-      </c>
-      <c r="J30" t="s">
-        <v>667</v>
-      </c>
-      <c r="K30" t="s">
-        <v>464</v>
-      </c>
-      <c r="L30" t="s">
-        <v>465</v>
-      </c>
-      <c r="O30" t="s">
-        <v>658</v>
-      </c>
-      <c r="P30" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>648</v>
-      </c>
-      <c r="B31" t="s">
-        <v>655</v>
-      </c>
-      <c r="C31">
-        <v>2017</v>
-      </c>
-      <c r="D31" t="s">
-        <v>157</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>669</v>
-      </c>
-      <c r="B32" t="s">
-        <v>655</v>
-      </c>
-      <c r="C32">
-        <v>2017</v>
-      </c>
-      <c r="D32" t="s">
-        <v>167</v>
-      </c>
-      <c r="E32" t="s">
-        <v>479</v>
-      </c>
-      <c r="F32" t="s">
-        <v>274</v>
-      </c>
-      <c r="G32" t="s">
-        <v>275</v>
-      </c>
-      <c r="H32" t="s">
-        <v>608</v>
-      </c>
-      <c r="I32" t="s">
-        <v>621</v>
-      </c>
-      <c r="J32" t="s">
-        <v>475</v>
-      </c>
-      <c r="K32" t="s">
-        <v>670</v>
-      </c>
-      <c r="L32" t="s">
-        <v>671</v>
-      </c>
-      <c r="M32" t="s">
-        <v>328</v>
-      </c>
-      <c r="O32" t="s">
-        <v>477</v>
-      </c>
-      <c r="P32" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>669</v>
-      </c>
-      <c r="B33" t="s">
-        <v>655</v>
-      </c>
-      <c r="C33">
-        <v>2017</v>
-      </c>
-      <c r="D33" t="s">
-        <v>167</v>
-      </c>
-      <c r="E33" t="s">
-        <v>474</v>
-      </c>
-      <c r="F33" t="s">
-        <v>274</v>
-      </c>
-      <c r="G33" t="s">
-        <v>275</v>
-      </c>
-      <c r="H33" t="s">
-        <v>608</v>
-      </c>
-      <c r="I33" t="s">
-        <v>621</v>
-      </c>
-      <c r="J33" t="s">
-        <v>475</v>
-      </c>
-      <c r="K33" t="s">
-        <v>476</v>
-      </c>
-      <c r="L33" t="s">
-        <v>671</v>
-      </c>
-      <c r="M33" t="s">
-        <v>328</v>
-      </c>
-      <c r="O33" t="s">
-        <v>477</v>
-      </c>
-      <c r="P33" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>672</v>
-      </c>
-      <c r="B34" t="s">
-        <v>655</v>
-      </c>
-      <c r="C34">
-        <v>2017</v>
-      </c>
-      <c r="D34" t="s">
-        <v>169</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>674</v>
-      </c>
-      <c r="B35" t="s">
-        <v>655</v>
-      </c>
-      <c r="C35">
-        <v>2017</v>
-      </c>
-      <c r="D35" t="s">
-        <v>177</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
-      <c r="R35" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>676</v>
-      </c>
-      <c r="B36" t="s">
-        <v>655</v>
-      </c>
-      <c r="C36">
-        <v>2016</v>
-      </c>
-      <c r="D36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E36" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="26"/>
-      <c r="Q36" s="26"/>
-      <c r="R36" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>648</v>
-      </c>
-      <c r="B37" t="s">
-        <v>655</v>
-      </c>
-      <c r="C37">
-        <v>2016</v>
-      </c>
-      <c r="D37" t="s">
-        <v>196</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="26"/>
-      <c r="Q37" s="26"/>
-      <c r="R37" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>672</v>
-      </c>
-      <c r="B38" t="s">
-        <v>655</v>
-      </c>
-      <c r="C38">
-        <v>2016</v>
-      </c>
-      <c r="D38" t="s">
-        <v>215</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>604</v>
-      </c>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
-      <c r="K38" s="26"/>
-      <c r="L38" s="26"/>
-      <c r="M38" s="26"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="26"/>
-      <c r="Q38" s="26"/>
-      <c r="R38" t="s">
-        <v>679</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="E34:Q34"/>
-    <mergeCell ref="E35:Q35"/>
-    <mergeCell ref="E36:Q36"/>
-    <mergeCell ref="E37:Q37"/>
-    <mergeCell ref="E38:Q38"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="E5:Q5"/>
-    <mergeCell ref="E6:Q6"/>
-    <mergeCell ref="E19:Q19"/>
-    <mergeCell ref="E24:Q24"/>
-    <mergeCell ref="E31:Q31"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="O2:Q2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="G2:H3 G7:H7 I11:I17 G18:H18 G20:H20 H23:I23 I21 H22">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Not sure"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="13">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="What is your decision about it?" prompt="Should we include this paper ? Why? Should we exclude it? Why? Any comments about the information extracted ?" sqref="A3" xr:uid="{B74B0685-CA13-44BA-A5D1-D5DF46E2780B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Who validated this paper?" prompt="Please write your name: Danny, Patrizio, Thorsten" sqref="B3" xr:uid="{2DEFEA2C-5473-4429-A6FC-045F9294E0FF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property Formalism" prompt="Mathematically based technique used to define the property.  E.g.  SetBased, State-Transition, Logics, Temporal Logic, Dynamic Logic, Other Logics, Process Algebra, Ontol-ogy" sqref="F3" xr:uid="{D77AEEA9-2595-4F02-8983-C41D9CB9B975}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property Language" prompt="Language used to specify the property.  E.g.  Computational Tree Logic(CTL), Linear-time Logic (LTL), Probabilistic Computational Tree Logic (PCTL)." sqref="G3" xr:uid="{0B8DCC9B-EAE6-49B2-84FA-4F3355DCA398}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Explicit time" prompt="Does the property explicitly specifies time?" sqref="H3" xr:uid="{E538F975-63E7-48B8-9F88-728733A97A0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Explicit probability" prompt="Does the property explicitly specifies probability?" sqref="I3" xr:uid="{AA968FDF-7F5D-4AD4-B1CC-D55F9520F62A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Target System" prompt="Whether  the  model  used  refers  to  the  target  system  behavior,  adaptation manager behavior, or other (environment)." sqref="L3" xr:uid="{6ED36671-A323-4902-9CB5-A5F2E5DD9E0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Model Type" prompt="Defines what is being modeled. E.g. Reliability, Performance, Functional behavior" sqref="M3" xr:uid="{4020A005-F7F5-45F8-B74A-8B4832C69B8F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Model Formalism" prompt="Mathematically based technique used to define the model.   E.g.   SetBased, State-Transition, Logics, Temporal Logic, Dynamic Logic, Other Logics, Process Algebra, Ontol-ogy" sqref="N3" xr:uid="{5FF34F97-89D5-4DBE-B3BF-CF74D8F2E0D8}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Use Case" prompt="Assurance provision method employed. Includes frameworks or techniques to provide assurance of correctness (verification, reasoning and synthesis). E.g. Model Checking, Theorem Proving, Runtime Monitoring, Assurance case synthesis, Synthesis of correct-by" sqref="O3" xr:uid="{D1A945E3-AA99-48B2-ACD3-8919483E9196}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Runtime" prompt=" Whether the approach is designed for offline or runtime. Offline techniques may be design-time or postmortem._x000a_" sqref="P3" xr:uid="{0D851ADF-7E2B-4A4D-A178-33D744F29896}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Applciation Domain" prompt=" Use case domain. E.g. Robotics, Self-Driving Vehicles, Internet of Things, Healthcare, Transportation, Mobile Communication, Finance, Business Analytics \&amp; eCommerce, Decision Support Systems, Forestry Farming \&amp; Urban Informatics, Manufacturing and Proc" sqref="Q3" xr:uid="{45708767-6543-43FE-B0A9-951696261A61}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property Extracted" prompt="The lower level of abstraction in which the extracted property categories" sqref="E3" xr:uid="{38A4DC14-B0DA-46F4-A40E-FABF3FE50921}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding aggregated data view for specification patterns
</commit_message>
<xml_diff>
--- a/Literature_review_data.xlsx
+++ b/Literature_review_data.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Razan\Bitbucket\mappingCTSEprops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F12E60-F454-46EF-B48E-82BC36AF95E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8882BD-AD3C-4A12-9F0A-FD7D0AABF3AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{93EA37D0-547C-4F6C-8D12-FC66693056E1}"/>
   </bookViews>
   <sheets>
     <sheet name="List of SEAMS publications" sheetId="1" r:id="rId1"/>
     <sheet name="Included papers extracted data" sheetId="2" r:id="rId2"/>
+    <sheet name="SE to specification patterns" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Included papers extracted data'!$A$1:$T$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'List of SEAMS publications'!$A$1:$E$119</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -129,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="599">
   <si>
     <t>ID</t>
   </si>
@@ -1926,6 +1930,15 @@
   </si>
   <si>
     <t>Safety (time constrained)</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of ID</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2084,6 +2097,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2121,6 +2142,1643 @@
   <person displayName="Ricardo" id="{A76E3C88-9401-4016-BAEC-8D918CBDCA0E}" userId="" providerId=""/>
   <person displayName="razan.ghzouli@chalmers.se" id="{5C2FDE4E-4832-4B34-ACD7-25B3303B9868}" userId="" providerId=""/>
 </personList>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Razan" refreshedDate="44238.634009837966" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="51" xr:uid="{A4957CF9-CD57-4EC4-ADF7-EC2BF1297B91}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:T52" sheet="Included papers extracted data"/>
+  </cacheSource>
+  <cacheFields count="20">
+    <cacheField name="Publication Year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2016" maxValue="2020"/>
+    </cacheField>
+    <cacheField name="ID" numFmtId="0">
+      <sharedItems count="22">
+        <s v="camara2:2020"/>
+        <s v="li:2020"/>
+        <s v="sakizloglou:2020"/>
+        <s v="shin:2020"/>
+        <s v="jamshidi:2019"/>
+        <s v="khakpour:2019"/>
+        <s v="solano:2019"/>
+        <s v="tsigkanos:2019"/>
+        <s v="devries:2018"/>
+        <s v="ductor:2018"/>
+        <s v="faccin:2018"/>
+        <s v="guerriero:2018"/>
+        <s v="marshall:2018"/>
+        <s v="olaechea:2018"/>
+        <s v="pournaras:2018"/>
+        <s v="rodrigues:2018"/>
+        <s v="cailliau:2017"/>
+        <s v="dasilva:2017"/>
+        <s v="moreno2:2017"/>
+        <s v="tahara:2017"/>
+        <s v="incerto:2016"/>
+        <s v="nahabedian:2016"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SE Property Extracted" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="SE Property Requirement" numFmtId="0">
+      <sharedItems count="15">
+        <s v="Time Related Property "/>
+        <s v="Performance"/>
+        <s v="Safety"/>
+        <s v="Resource Usage"/>
+        <s v="Security"/>
+        <s v="Reliability"/>
+        <s v="Availability"/>
+        <s v="Accessibility"/>
+        <s v="Functional"/>
+        <s v="Recovery"/>
+        <s v="Privacy"/>
+        <s v="Adaptation"/>
+        <s v="Deadlock-Freedom"/>
+        <s v="Safety (time constrained)"/>
+        <s v="User Properties"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SE Property Specification" numFmtId="0">
+      <sharedItems count="7">
+        <s v="Cost/Reward"/>
+        <s v="Reachability"/>
+        <s v="Liveness"/>
+        <s v="Fitness Function"/>
+        <s v="Static Property"/>
+        <s v="Safety"/>
+        <s v="Fairness"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="SE Property Formalism" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="SE Property Language" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Explicit time" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Explicit probability" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Formula (optional)" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Statement (optional)" numFmtId="0">
+      <sharedItems containsBlank="1" longText="1"/>
+    </cacheField>
+    <cacheField name="Target System" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Model Type" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Model Formalism" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Use Case" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Runtime" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Application Domain" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Category (According to ps paterns)" numFmtId="0">
+      <sharedItems count="15">
+        <s v="NA"/>
+        <s v="Globally Probabilistic Existence"/>
+        <s v="Globally Timed Precedence"/>
+        <s v="Globally Timed Existence"/>
+        <s v="Globally Timed Response"/>
+        <s v="Globally Untimed Universality"/>
+        <s v="Globally Timed Response Chain"/>
+        <s v="Globally Untimed Response"/>
+        <s v="Globally Timed Universality"/>
+        <s v="Globally Untimed Existence"/>
+        <s v="Globally Untimed Precedence Chain"/>
+        <s v="Globally Untimed Absence"/>
+        <s v="Globally Probabilistic Timed Response"/>
+        <s v="After Probabilistic Timed Absence"/>
+        <s v="Globally Probabilistic Untimed Until, with P negated"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Reason for No PS pattern" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Category (According to control paterns)" numFmtId="0">
+      <sharedItems count="4">
+        <s v="NA"/>
+        <s v="Settling Time"/>
+        <s v="Stability"/>
+        <s v="Overshoot"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="51">
+  <r>
+    <n v="2020"/>
+    <x v="0"/>
+    <s v="Cost/Reward"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="R{time}min=? [F goal]"/>
+    <s v="&quot;Time to target location.&quot; [Table 2]"/>
+    <s v="Target system behavior"/>
+    <s v="Software Components + Energy Cost"/>
+    <s v="Probabilistic model"/>
+    <s v="Quantitative synthesis and verification of  an approach that consider the impact of mutual dependencies of software architcture and task planning_x000a_on the satisfaction of mission goals."/>
+    <s v="Runtime"/>
+    <s v="Robotics (mission planning)"/>
+    <x v="0"/>
+    <s v="reward quantifier"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="0"/>
+    <s v="Cost/Reward"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="R{energy}max=?  [F goal]"/>
+    <s v="&quot;Remaining energy at target location.&quot; [Table 2]"/>
+    <s v="Target system behavior"/>
+    <s v="Software Components + Energy Cost"/>
+    <s v="Probabilistic model"/>
+    <s v="Quantitative synthesis and verification of  an approach that consider the impact of mutual dependencies of software architcture and task planning_x000a_on the satisfaction of mission goals."/>
+    <s v="Runtime"/>
+    <s v="Robotics (mission planning)"/>
+    <x v="0"/>
+    <s v="reward quantifier"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="0"/>
+    <s v="Reachability"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="Pmax=?[F (goal ∧ ¬collided)]"/>
+    <s v="&quot;Non-collision probability.&quot; [Table 2]"/>
+    <s v="Target system behavior"/>
+    <s v="Software Components + Energy Cost"/>
+    <s v="Probabilistic model"/>
+    <s v="Quantitative synthesis and verification of  an approach that consider the impact of mutual dependencies of software architcture and task planning_x000a_on the satisfaction of mission goals."/>
+    <s v="Runtime"/>
+    <s v="Robotics (mission planning)"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="1"/>
+    <s v="Cost/Reward"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="R{utility}max=? [Fc end]"/>
+    <s v="Minimize cost of providing useful information to the human on the loop (Section 3.3)"/>
+    <s v="Adaptation Manager (Human)"/>
+    <s v="Human behavior and machine behavior"/>
+    <s v="Probabilistic model"/>
+    <s v="Synthesis (The use of probabilistic model checking to perform the synthesis of optimal explanations)"/>
+    <s v="Offline"/>
+    <s v="Autonomous Vehicle (Autonomous Driving Systems)"/>
+    <x v="0"/>
+    <s v="reward quantifier"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="2"/>
+    <s v="Safety"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="MTGL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="𝜙 = ∀N 𝜙1 → ♦[0,3600]∃ 𝜙2"/>
+    <s v="“If a patient has undergone a procedure” and “an antibiotic has not been administered up until 1 hour before the procedure” respectively (Section 3.2)"/>
+    <s v="Target system behavior"/>
+    <s v="Architecture"/>
+    <s v="Graph-based"/>
+    <s v="Verification of an approach to identify adoptation issues "/>
+    <s v="Runtime"/>
+    <s v="IoT (Healthcare)"/>
+    <x v="2"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="3"/>
+    <s v="Cost"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="eq 2"/>
+    <s v="Adaptation cost (Section 3.3)"/>
+    <s v="Adaptation Manager"/>
+    <s v="Performance"/>
+    <s v="Graph-based"/>
+    <s v="&quot;The “analyze” step is in charge of determining whether, or not, the network is congested&quot; (Optimization)"/>
+    <s v="Runtime"/>
+    <s v="IoT (SDN)"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="3"/>
+    <s v="Delay"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="eq 3"/>
+    <s v="Data transmisison delay (Section 3.3)"/>
+    <s v="Target system behavior"/>
+    <s v="Performance"/>
+    <s v="Graph-based"/>
+    <s v="&quot;The “analyze” step is in charge of determining whether, or not, the network is congested&quot; (Optimization)"/>
+    <s v="Runtime"/>
+    <s v="IoT (SDN)"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="3"/>
+    <s v="Utilization"/>
+    <x v="3"/>
+    <x v="3"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="eq 1"/>
+    <s v="Minimize Link utilization (Section 3.3)"/>
+    <s v="Target system behavior"/>
+    <s v="Performance"/>
+    <s v="Graph-based"/>
+    <s v="&quot;The “analyze” step is in charge of determining whether, or not, the network is congested&quot; (Optimization)"/>
+    <s v="Runtime"/>
+    <s v="IoT (SDN)"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="4"/>
+    <s v="Cost/Reward"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Eq 4"/>
+    <s v="&quot;Time to target location&quot;"/>
+    <s v="Target system behavior + Environment"/>
+    <s v="Functional behavior"/>
+    <s v="Probabilistic model"/>
+    <s v="Task plan Synthesis (MC)"/>
+    <s v="Runtime"/>
+    <s v="Robotics (mission planning)"/>
+    <x v="3"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="5"/>
+    <s v="Attack Graph Probability"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="Table II"/>
+    <s v="&quot;Average attacker graph probability of all attackers goals&quot; &quot;represents the probability of reaching a specific node in the attack graph via several multi-step attack&quot;"/>
+    <s v="Adaptation Manager"/>
+    <s v="Security (attack graph)"/>
+    <s v="Graph-based"/>
+    <s v="Analyse risk of adaptation"/>
+    <s v="Runtime"/>
+    <s v="Webservice based (ZNN)"/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="5"/>
+    <s v="Length of attack paths "/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <m/>
+    <s v="&quot;Average Length of Attack paths to attackers goal&quot;"/>
+    <s v="Adaptation Manager"/>
+    <s v="Security (attack graph)"/>
+    <s v="Graph-based"/>
+    <s v="Analyse risk of adaptation"/>
+    <s v="Runtime"/>
+    <s v="Webservice based (ZNN)"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="5"/>
+    <s v="Number of Attack paths"/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <m/>
+    <s v="&quot;Number of attacker paths&quot;"/>
+    <s v="Adaptation Manager"/>
+    <s v="Security (attack graph)"/>
+    <s v="Graph-based"/>
+    <s v="Analyse risk of adaptation"/>
+    <s v="Runtime"/>
+    <s v="Webservice based (ZNN)"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="6"/>
+    <s v="Reachability"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Table II"/>
+    <s v="&quot;In this work, we focus on reliability and cost properties. Their specifications are based on the idea of the probabilistic existence property [26], that is, the probability that a system will eventually reach a state that satisfies a goal of interest&quot;"/>
+    <s v="Target system behavior + Environment"/>
+    <s v="Functional behavior"/>
+    <s v="Probabilistic model"/>
+    <s v="Adaptation Policy Synthesis (ad hoc)"/>
+    <s v="Offline"/>
+    <s v="Health Care "/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="6"/>
+    <s v="Reliability"/>
+    <x v="5"/>
+    <x v="1"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="Table II"/>
+    <s v="&quot;In this work, we focus on reliability and cost properties. Their specifications are based on the idea of the probabilistic existence property [26], that is, the probability that a system will eventually reach a state that satisfies a goal of interest&quot;"/>
+    <s v="Target system behavior + Environment"/>
+    <s v="Functional behavior"/>
+    <s v="Probabilistic model"/>
+    <s v="Adaptation Policy Synthesis (ad hoc)"/>
+    <s v="Offline"/>
+    <s v="Health Care "/>
+    <x v="1"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="7"/>
+    <s v="Availability"/>
+    <x v="6"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="STREL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Sect V"/>
+    <s v="&quot;Each hospital has a taxi less than 10 minutes away&quot;"/>
+    <s v="Environment"/>
+    <s v="Accessibility Spatial Model"/>
+    <s v="Graph-based"/>
+    <s v="Verification of spatial and time constrained properties"/>
+    <s v="Runtime"/>
+    <s v="IoT (trajectory tracing)"/>
+    <x v="4"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="7"/>
+    <s v="Complex Spatial Relationship"/>
+    <x v="7"/>
+    <x v="1"/>
+    <s v="Temporal Logic"/>
+    <s v="STREL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Sect V"/>
+    <s v="&quot;Taxis should be at landmarks where one can reach the main square through bus or metro stops in less than 10 minutes&quot;"/>
+    <s v="Environment"/>
+    <s v="Accessibility Spatial Model"/>
+    <s v="Graph-based"/>
+    <s v="Verification of spatial and time constrained properties"/>
+    <s v="Runtime"/>
+    <s v="IoT (trajectory tracing)"/>
+    <x v="5"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="7"/>
+    <s v="Liveness"/>
+    <x v="7"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="STREL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Sect V"/>
+    <s v="&quot;If there is a landmark where more than 200 people are located, then a taxi will be there within 20 minutes”"/>
+    <s v="Environment"/>
+    <s v="Accessibility Spatial Model"/>
+    <s v="Graph-based"/>
+    <s v="Verification of spatial and time constrained properties"/>
+    <s v="Runtime"/>
+    <s v="IoT (trajectory tracing)"/>
+    <x v="4"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="8"/>
+    <s v="Feature Interaction"/>
+    <x v="8"/>
+    <x v="4"/>
+    <s v="Boolean Expression"/>
+    <s v="FOL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 3.2 exmpl"/>
+    <s v="&quot;Maintain Break System&quot; &quot; F is the set of features in the feature set that satisfies (FB ∨ FC) ∧ (FD ∨ FE)&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <m/>
+    <s v="Generate Runtime Monitors for Feature Interaction Detection"/>
+    <s v="Runtime"/>
+    <s v="Autonomous Vehicle (Automotive Braking System)"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="9"/>
+    <s v="Reliability"/>
+    <x v="5"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Equation 3"/>
+    <s v="&quot;Guarantee of continuity of computation w.r.t the agents criticalities&quot;Section 3.3"/>
+    <s v="Target system behavior"/>
+    <s v="Agents Allocation"/>
+    <s v="Graph-based"/>
+    <s v="Validation of adaptive replication"/>
+    <s v="Runtime"/>
+    <s v="Multi agents system"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="9"/>
+    <s v="Resource Usage"/>
+    <x v="3"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Equation 4"/>
+    <s v="&quot;Processor use rate(overloaded)&quot; Section 3.2"/>
+    <s v="Target system behavior"/>
+    <s v="Agents Allocation"/>
+    <s v="Graph-based"/>
+    <s v="Validation of adaptive replication"/>
+    <s v="Runtime"/>
+    <s v="Multi agents system"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="9"/>
+    <s v="Resource Usage"/>
+    <x v="3"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Equation 4"/>
+    <s v="&quot;Memory use rate(overloaded)&quot; Section 3.2"/>
+    <s v="Target system behavior"/>
+    <s v="Agents Allocation"/>
+    <s v="Graph-based"/>
+    <s v="Validation of adaptive replication"/>
+    <s v="Runtime"/>
+    <s v="Multi agents system"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="10"/>
+    <s v="Structural Property"/>
+    <x v="9"/>
+    <x v="4"/>
+    <s v="Boolean Expression"/>
+    <s v="FOL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <m/>
+    <m/>
+    <s v="Target system behavior"/>
+    <s v="BDI Architecture"/>
+    <s v="NA"/>
+    <s v="Reverting actions"/>
+    <s v="Offline"/>
+    <s v="Smart Homes"/>
+    <x v="0"/>
+    <s v="complex formulation"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="11"/>
+    <s v="Privacy"/>
+    <x v="10"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="MTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Eq 8 (if else)"/>
+    <s v="&quot;if someone from MarketConsult is observing S4 with the purpose of doing some analytics, then tuples referring to Bob have to be evicted from the input of the operator that produces S4&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Behavioral model"/>
+    <s v="Rewriting of operators to enforce policies"/>
+    <s v="Runtime"/>
+    <s v="e-Commerce &amp; Financial"/>
+    <x v="6"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="11"/>
+    <s v="Privacy"/>
+    <x v="10"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="MTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Eq (7) A and B or C implies not (X)"/>
+    <s v="&quot;given a tuple t ∈ S3 which refers to Bob, if (i) the S3 observer is an employee of MarketConsult with the purpose of doing analytics and (ii) there has been a tuple in t ∈ S2 during the last 30 minutes such that t.nT ransactions was greater than 3 and (iii) the field t.amount is greater than 100, then the generalization vector (0, 1) has to be applied to t, i.e., the field t.dataSubject has to be left as it is, while the field t.totalAmount has to be generalized to level 1 of its DGH.&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Behavioral model"/>
+    <s v="Rewriting of operators to enforce policies"/>
+    <s v="Runtime"/>
+    <s v="e-Commerce &amp; Financial"/>
+    <x v="7"/>
+    <s v="NA"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="12"/>
+    <s v="Liveness"/>
+    <x v="4"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 3.2. R4"/>
+    <s v="&quot;All audit records are sent to the audit trail (AU-12(1))&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Proof-based"/>
+    <s v="Certification of security controls through verification of auditing process"/>
+    <s v="Offline"/>
+    <s v="Security Control (Inventory’s stock condition tracking)"/>
+    <x v="7"/>
+    <s v="NA"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="12"/>
+    <s v="Liveness"/>
+    <x v="4"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 3.2. R2"/>
+    <s v="&quot;For each predefined auditable event, an audit record satisfying the minimal contents is generated when an auditable event occurs (AU-12c, AU-2d, AU-3)&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Proof-based"/>
+    <s v="Certification of security controls through verification of auditing process"/>
+    <s v="Offline"/>
+    <s v="Security Control (Inventory’s stock condition tracking)"/>
+    <x v="7"/>
+    <s v="NA"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="12"/>
+    <s v="Safety"/>
+    <x v="4"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Sect 3.2. R5"/>
+    <s v="&quot;The audit trail time-correlates the audit records (AU-12(1))&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Proof-based"/>
+    <s v="Certification of security controls through verification of auditing process"/>
+    <s v="Offline"/>
+    <s v="Security Control (Inventory’s stock condition tracking)"/>
+    <x v="8"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="12"/>
+    <s v="Time Constraint"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Sect 3.2. R6"/>
+    <s v="&quot;Time correlation is checked against a defined level of tolerance (AU-12(1)&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Proof-based"/>
+    <s v="Certification of security controls through verification of auditing process"/>
+    <s v="Offline"/>
+    <s v="Security Control (Inventory’s stock condition tracking)"/>
+    <x v="9"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="12"/>
+    <s v="User Properties"/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 3.2. R1"/>
+    <s v="&quot;For each component (C) in the information system (IS) identified to have auditable events, there exists a function to perform auditing for predefined auditable events (AU-12a, AU-2a)&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Proof-based"/>
+    <s v="Certification of security controls through verification of auditing process"/>
+    <s v="Offline"/>
+    <s v="Security Control (Inventory’s stock condition tracking)"/>
+    <x v="5"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="12"/>
+    <s v="User Properties"/>
+    <x v="4"/>
+    <x v="4"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 3.2. R3"/>
+    <s v="&quot;There exists a system-wide, virtual or physical component, which we will call Audit , that collects auditable events (AU-12(1)) from designated components.&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Proof-based"/>
+    <s v="Certification of security controls through verification of auditing process"/>
+    <s v="Offline"/>
+    <s v="Security Control (Inventory’s stock condition tracking)"/>
+    <x v="9"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="13"/>
+    <s v="Functional Behavior"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Boolean Expression"/>
+    <s v="FOL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="(sdst ,γ ∧γ (t),r +W (t)),  where CV ∧ ¬GPS must hold with accumulated rewards"/>
+    <s v="Section 4.1"/>
+    <s v="Target system behavior"/>
+    <s v="Feature model"/>
+    <s v="Graph-based"/>
+    <s v="Quality of service estimation for DSPL configurations; Simultaneous analses of the family of products to speed up the analysis."/>
+    <s v="Runtime"/>
+    <s v="Autonomous Vehicle (Unmanned Aerial Vehicle)"/>
+    <x v="5"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="14"/>
+    <s v="Failure management"/>
+    <x v="11"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="Yes"/>
+    <s v="Yes"/>
+    <s v="eq 1"/>
+    <s v="&quot;The damage spread concerns the probability of decreasing the links survivability over the iterations of the cascading failure.&quot;"/>
+    <s v="Adaptation Manager"/>
+    <s v="Cascading Failures Mathematical Framework"/>
+    <s v="Algebraic"/>
+    <s v="Interdependent power networks planning, regulation"/>
+    <s v="Offline"/>
+    <s v="Power networks"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="14"/>
+    <s v="Failure management"/>
+    <x v="11"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="Yes"/>
+    <s v="Yes"/>
+    <s v="eq 2"/>
+    <s v="&quot;The power cascade ct concerns the probability of progressing the iteration of the cascading failure. &quot;"/>
+    <s v="Adaptation Manager"/>
+    <s v="Cascading Failures Mathematical Framework"/>
+    <s v="Algebraic"/>
+    <s v="Interdependent power networks planning, regulation"/>
+    <s v="Offline"/>
+    <s v="Power networks"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="14"/>
+    <s v="Failure management"/>
+    <x v="11"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 4.2"/>
+    <s v="&quot;The damage correlation rt (si,t , sj,t ) measures the Pearson correlation coefficient between the status of the links si,t and sj,t after the removal of link i and j respectively,&quot;"/>
+    <s v="Adaptation Manager"/>
+    <s v="Cascading Failures Mathematical Framework"/>
+    <s v="Algebraic"/>
+    <s v="Interdependent power networks planning, regulation"/>
+    <s v="Offline"/>
+    <s v="Power networks"/>
+    <x v="0"/>
+    <s v="No notion of time or order between states/events"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="15"/>
+    <s v="Fairness"/>
+    <x v="0"/>
+    <x v="6"/>
+    <s v="Temporal Logic"/>
+    <s v="TCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Table 3.P2"/>
+    <s v="&quot;Scheduling period&quot; Section 3.1.1"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Assurance of self-adaptive systems"/>
+    <s v="Offline"/>
+    <s v="Health Care"/>
+    <x v="10"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="15"/>
+    <s v="Monitored values"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="TCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Table 3.P7"/>
+    <s v="&quot;Patient status monitored&quot;  Section 3.1.1"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Assurance of self-adaptive systems"/>
+    <s v="Offline"/>
+    <s v="Health Care"/>
+    <x v="7"/>
+    <s v="NA"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="15"/>
+    <s v="Monitored values"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="TCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v=" Table 3.P8"/>
+    <s v="&quot;Vital signs monitored&quot; Section 3.1.1"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Assurance of self-adaptive systems"/>
+    <s v="Offline"/>
+    <s v="Health Care"/>
+    <x v="7"/>
+    <s v="NA"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="15"/>
+    <s v="Monitored values"/>
+    <x v="5"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="TCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Table 3.P9,P10"/>
+    <s v="&quot;Vital signs analyzed&quot;  Section 3.1.1"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Assurance of self-adaptive systems"/>
+    <s v="Offline"/>
+    <s v="Health Care"/>
+    <x v="7"/>
+    <s v="NA"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="15"/>
+    <s v="Safety"/>
+    <x v="12"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="TCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Table 3.P1"/>
+    <s v="&quot;Deadlock freedom&quot; Section 3.1.1"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Assurance of self-adaptive systems"/>
+    <s v="Offline"/>
+    <s v="Health Care"/>
+    <x v="11"/>
+    <s v="NA"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="15"/>
+    <s v="Safety"/>
+    <x v="11"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="TCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Table 3. P4,P5,P6"/>
+    <s v="Section 3.1.1"/>
+    <s v="Adaptation Manager"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Assurance of self-adaptive systems"/>
+    <s v="Offline"/>
+    <s v="Health Care"/>
+    <x v="5"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="15"/>
+    <s v="Time Constraint"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="TCTL"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Table 3.P3"/>
+    <s v="&quot;An Emergency will be detected within a Detection Time Constraint&quot; Section 3.1.1"/>
+    <s v="Target system behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Assurance of self-adaptive systems"/>
+    <s v="Offline"/>
+    <s v="Health Care"/>
+    <x v="5"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="16"/>
+    <s v="Reachability"/>
+    <x v="8"/>
+    <x v="1"/>
+    <s v="Temporal Logic"/>
+    <s v="MTL"/>
+    <s v="Yes"/>
+    <s v="Yes"/>
+    <s v="Sect IV.A."/>
+    <s v="&quot;Local warned when levels critical&quot;"/>
+    <s v="Target system behavior + Environment"/>
+    <s v="Degree of Satisfaction"/>
+    <s v="Graph-based"/>
+    <s v="Runtime monitoring obstacles and the probability to reach or maintain a goal"/>
+    <s v="Runtime"/>
+    <s v="Health Care / Transportation"/>
+    <x v="12"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="16"/>
+    <s v="Safety"/>
+    <x v="13"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="MTL"/>
+    <s v="Yes"/>
+    <s v="Yes"/>
+    <s v="Sect IV.A."/>
+    <m/>
+    <s v="Target system behavior + Environment"/>
+    <s v="Degree of Satisfaction"/>
+    <s v="Graph-based"/>
+    <s v="Runtime monitoring obstacles and the probability to reach or maintain a goal"/>
+    <s v="Runtime"/>
+    <s v="Health Care / Transportation"/>
+    <x v="13"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="17"/>
+    <s v="Reachability"/>
+    <x v="14"/>
+    <x v="0"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Table 2.P1,P2,P5,P6"/>
+    <s v="Section 4.C"/>
+    <s v="Human behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Adaptation recommendation"/>
+    <s v="Runtime"/>
+    <s v="Information System"/>
+    <x v="0"/>
+    <s v="reward quantifier"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="17"/>
+    <s v="User Properties"/>
+    <x v="14"/>
+    <x v="4"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="Table 2.P3"/>
+    <s v="&quot;Support users that cancel tickets Support without requiring more information&quot; Section 4.C"/>
+    <s v="Human behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Adaptation recommendation"/>
+    <s v="Runtime"/>
+    <s v="Information System"/>
+    <x v="14"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="17"/>
+    <s v="User Properties"/>
+    <x v="14"/>
+    <x v="4"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="Table 2.P4"/>
+    <s v="&quot;Support users that open tickets on behalf of clients where the ticket is subsequently abandoned&quot; Section 4.C"/>
+    <s v="Human behavior"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Adaptation recommendation"/>
+    <s v="Runtime"/>
+    <s v="Information System"/>
+    <x v="14"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="18"/>
+    <s v="Delayed Reachability"/>
+    <x v="8"/>
+    <x v="1"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="Sect III.B"/>
+    <s v="&quot;indicates that if the system is in configuration c, with the passage of one decision interval it will reach configuration c_x0002_&quot;"/>
+    <s v="Target system behavior + Environment"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Adaptation tactic synthesis"/>
+    <s v="Offline"/>
+    <s v="Unmanned Aerial Vehicle"/>
+    <x v="4"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="18"/>
+    <s v="Immediate Reachability"/>
+    <x v="8"/>
+    <x v="1"/>
+    <s v="Temporal Logic"/>
+    <s v="PCTL"/>
+    <s v="No"/>
+    <s v="Yes"/>
+    <s v="Sect III.B"/>
+    <s v="&quot;Indicates that configuration c can be reached immediately from c through the use of an adaptation action&quot;"/>
+    <s v="Target system behavior + Environment"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Adaptation tactic synthesis"/>
+    <s v="Offline"/>
+    <s v="Unmanned Aerial Vehicle"/>
+    <x v="4"/>
+    <s v="NA"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="19"/>
+    <s v="Liveness"/>
+    <x v="8"/>
+    <x v="2"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 3.D"/>
+    <m/>
+    <s v="Adaptation Manager"/>
+    <s v="Functional behavior"/>
+    <s v="UML"/>
+    <s v="Verification (model checking) of dynamic evolution using dynamic aspects"/>
+    <s v="NA"/>
+    <s v="Health Care (service)"/>
+    <x v="7"/>
+    <s v="NA"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2016"/>
+    <x v="20"/>
+    <s v="Time Constraint"/>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Algebraic"/>
+    <s v="Algebra"/>
+    <s v="Yes"/>
+    <s v="No"/>
+    <s v="Sect 4.2"/>
+    <s v="&quot;it is worth to point out that our utilization constraint can be interpreted as a QoS requirement related to energy efficiency by relating servers utilization to energy consumption&quot;"/>
+    <s v="Target system behavior"/>
+    <s v="Performance"/>
+    <s v="Algebraic"/>
+    <s v="Symbolic analysis"/>
+    <s v="Offline"/>
+    <s v="Load Balancing System"/>
+    <x v="8"/>
+    <s v="NA"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2016"/>
+    <x v="21"/>
+    <s v="Correct update"/>
+    <x v="11"/>
+    <x v="5"/>
+    <s v="Temporal Logic"/>
+    <s v="LTL"/>
+    <s v="No"/>
+    <s v="No"/>
+    <s v="Sect 4.3"/>
+    <s v="&quot;T is a safety property then Gu can be encoded as an obligation property&quot;"/>
+    <s v="Adaptation Manager + Environment"/>
+    <s v="Functional behavior"/>
+    <s v="Graph-based"/>
+    <s v="Synthesis for safe runtime update of controllers"/>
+    <s v="Runtime"/>
+    <s v="Industrial Automation "/>
+    <x v="0"/>
+    <s v="complex formulation"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{418EC6DB-CD6B-47AF-ACDE-794ECE5C8374}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B81" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="20">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="23">
+        <item x="16"/>
+        <item x="0"/>
+        <item x="17"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="20"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="18"/>
+        <item x="21"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="19"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="16">
+        <item x="7"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="13"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="14"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="17"/>
+    <field x="4"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="78">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ID" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4510,9 +6168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CCF711-4516-4809-827A-2B0BF844EAD5}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:S1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7763,4 +9419,655 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838DE3DA-E6C5-4B3E-94A1-AE1516DA5380}">
+  <dimension ref="A3:B81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>596</v>
+      </c>
+      <c r="B3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="B4" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B14" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B17" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B18" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B20" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="B24" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B26" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="B27" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="B29" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="B32" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B34" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B35" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B37" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B39" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B40" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B42" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B43" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B45" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B47" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="22" t="s">
+        <v>432</v>
+      </c>
+      <c r="B48" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B50" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="B51" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B55" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="B57" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B58" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="B60" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B62" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B64" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" s="24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B67" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="B71" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B73" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B74" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B75" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="B81" s="24">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>